<commit_message>
fix akurasi yg salah
</commit_message>
<xml_diff>
--- a/TA bab 1-4/uji 100x belajar aimdata graphic.xlsx
+++ b/TA bab 1-4/uji 100x belajar aimdata graphic.xlsx
@@ -35,13 +35,13 @@
     <t>My Bot 3</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>GamePlay</t>
   </si>
   <si>
     <t>reward</t>
-  </si>
-  <si>
-    <t>gameplay</t>
   </si>
 </sst>
 </file>
@@ -131,8 +131,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>My Bot 1</a:t>
+              <a:t>My</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Bot 1</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -244,34 +249,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>788.63</c:v>
+                  <c:v>404.72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>214.36</c:v>
+                  <c:v>1439.74</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>468.44</c:v>
+                  <c:v>1728.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1500.49</c:v>
+                  <c:v>2017.33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1731.31</c:v>
+                  <c:v>1088.4000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>606.62</c:v>
+                  <c:v>1223.73</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>593.95000000000005</c:v>
+                  <c:v>1109.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>191.75</c:v>
+                  <c:v>935.17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1297.08</c:v>
+                  <c:v>400.62</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>418.87</c:v>
+                  <c:v>326.02999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -279,7 +284,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BA9B-4738-A5EA-F2C0ABB2A25F}"/>
+              <c16:uniqueId val="{00000000-778D-4396-AC86-82D7543A48F0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -292,11 +297,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="680295488"/>
-        <c:axId val="680290080"/>
+        <c:axId val="1840463072"/>
+        <c:axId val="1840470144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="680295488"/>
+        <c:axId val="1840463072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -339,7 +344,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="680290080"/>
+        <c:crossAx val="1840470144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -347,7 +352,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="680290080"/>
+        <c:axId val="1840470144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +403,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="680295488"/>
+        <c:crossAx val="1840463072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -482,11 +487,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>My</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Bot 2</a:t>
+              <a:t>My Bot 2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -599,34 +600,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1271</c:v>
+                  <c:v>1163.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1174</c:v>
+                  <c:v>1474.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1064.21</c:v>
+                  <c:v>1594</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1168</c:v>
+                  <c:v>1059</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1381.85</c:v>
+                  <c:v>1489.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>953</c:v>
+                  <c:v>1464.09</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1172.45</c:v>
+                  <c:v>1488</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>953</c:v>
+                  <c:v>1582.45</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1593.83</c:v>
+                  <c:v>1391</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1267.43</c:v>
+                  <c:v>1396.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -634,7 +635,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6ADF-4C24-97AF-DA09ABB6BEE2}"/>
+              <c16:uniqueId val="{00000000-6EDD-422D-9FD7-4F76C65262C2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -647,11 +648,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="680293408"/>
-        <c:axId val="680295072"/>
+        <c:axId val="1832547344"/>
+        <c:axId val="1832548592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="680293408"/>
+        <c:axId val="1832547344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,7 +695,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="680295072"/>
+        <c:crossAx val="1832548592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -702,7 +703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="680295072"/>
+        <c:axId val="1832548592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,7 +754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="680293408"/>
+        <c:crossAx val="1832547344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -950,34 +951,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1615.4</c:v>
+                  <c:v>2007.96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2210.7399999999998</c:v>
+                  <c:v>856.26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2158.5700000000002</c:v>
+                  <c:v>337.97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1164.58</c:v>
+                  <c:v>820.56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>639.72</c:v>
+                  <c:v>1125.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2066.5500000000002</c:v>
+                  <c:v>1106.28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2182.63</c:v>
+                  <c:v>1055.42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2343.92</c:v>
+                  <c:v>1168.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>897.34</c:v>
+                  <c:v>1907.24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1961.51</c:v>
+                  <c:v>1716.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -985,7 +986,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F757-40BB-96B9-88C97346C988}"/>
+              <c16:uniqueId val="{00000000-B9A9-45C5-9A00-F7204D43EE43}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -998,11 +999,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="670469472"/>
-        <c:axId val="670471552"/>
+        <c:axId val="1828896400"/>
+        <c:axId val="1828890160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="670469472"/>
+        <c:axId val="1828896400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1046,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="670471552"/>
+        <c:crossAx val="1828890160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1053,7 +1054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="670471552"/>
+        <c:axId val="1828890160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1104,7 +1105,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="670469472"/>
+        <c:crossAx val="1828896400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2826,19 +2827,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2855,20 +2856,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:colOff>338137</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2886,19 +2887,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>328612</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3181,8 +3182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3192,28 +3193,28 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
         <v>5</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
@@ -3224,7 +3225,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>788.63</v>
+        <v>404.72</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -3233,7 +3234,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1271</v>
+        <v>1163.02</v>
       </c>
       <c r="J2" t="s">
         <v>2</v>
@@ -3242,7 +3243,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>1615.4</v>
+        <v>2007.96</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -3253,7 +3254,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>214.36</v>
+        <v>1439.74</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -3262,7 +3263,7 @@
         <v>2</v>
       </c>
       <c r="H3">
-        <v>1174</v>
+        <v>1474.4</v>
       </c>
       <c r="J3" t="s">
         <v>2</v>
@@ -3271,7 +3272,7 @@
         <v>2</v>
       </c>
       <c r="L3">
-        <v>2210.7399999999998</v>
+        <v>856.26</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -3282,7 +3283,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>468.44</v>
+        <v>1728.6</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
@@ -3291,7 +3292,7 @@
         <v>3</v>
       </c>
       <c r="H4">
-        <v>1064.21</v>
+        <v>1594</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
@@ -3300,7 +3301,7 @@
         <v>3</v>
       </c>
       <c r="L4">
-        <v>2158.5700000000002</v>
+        <v>337.97</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -3311,7 +3312,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>1500.49</v>
+        <v>2017.33</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
@@ -3320,7 +3321,7 @@
         <v>4</v>
       </c>
       <c r="H5">
-        <v>1168</v>
+        <v>1059</v>
       </c>
       <c r="J5" t="s">
         <v>2</v>
@@ -3329,7 +3330,7 @@
         <v>4</v>
       </c>
       <c r="L5">
-        <v>1164.58</v>
+        <v>820.56</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -3340,7 +3341,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>1731.31</v>
+        <v>1088.4000000000001</v>
       </c>
       <c r="F6" t="s">
         <v>1</v>
@@ -3349,7 +3350,7 @@
         <v>5</v>
       </c>
       <c r="H6">
-        <v>1381.85</v>
+        <v>1489.48</v>
       </c>
       <c r="J6" t="s">
         <v>2</v>
@@ -3358,7 +3359,7 @@
         <v>5</v>
       </c>
       <c r="L6">
-        <v>639.72</v>
+        <v>1125.48</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -3369,7 +3370,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>606.62</v>
+        <v>1223.73</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
@@ -3378,7 +3379,7 @@
         <v>6</v>
       </c>
       <c r="H7">
-        <v>953</v>
+        <v>1464.09</v>
       </c>
       <c r="J7" t="s">
         <v>2</v>
@@ -3387,7 +3388,7 @@
         <v>6</v>
       </c>
       <c r="L7">
-        <v>2066.5500000000002</v>
+        <v>1106.28</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -3398,7 +3399,7 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>593.95000000000005</v>
+        <v>1109.2</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
@@ -3407,7 +3408,7 @@
         <v>7</v>
       </c>
       <c r="H8">
-        <v>1172.45</v>
+        <v>1488</v>
       </c>
       <c r="J8" t="s">
         <v>2</v>
@@ -3416,7 +3417,7 @@
         <v>7</v>
       </c>
       <c r="L8">
-        <v>2182.63</v>
+        <v>1055.42</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -3427,7 +3428,7 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>191.75</v>
+        <v>935.17</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
@@ -3436,7 +3437,7 @@
         <v>8</v>
       </c>
       <c r="H9">
-        <v>953</v>
+        <v>1582.45</v>
       </c>
       <c r="J9" t="s">
         <v>2</v>
@@ -3445,7 +3446,7 @@
         <v>8</v>
       </c>
       <c r="L9">
-        <v>2343.92</v>
+        <v>1168.5</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -3456,7 +3457,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>1297.08</v>
+        <v>400.62</v>
       </c>
       <c r="F10" t="s">
         <v>1</v>
@@ -3465,7 +3466,7 @@
         <v>9</v>
       </c>
       <c r="H10">
-        <v>1593.83</v>
+        <v>1391</v>
       </c>
       <c r="J10" t="s">
         <v>2</v>
@@ -3474,7 +3475,7 @@
         <v>9</v>
       </c>
       <c r="L10">
-        <v>897.34</v>
+        <v>1907.24</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -3485,7 +3486,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>418.87</v>
+        <v>326.02999999999997</v>
       </c>
       <c r="F11" t="s">
         <v>1</v>
@@ -3494,7 +3495,7 @@
         <v>10</v>
       </c>
       <c r="H11">
-        <v>1267.43</v>
+        <v>1396.81</v>
       </c>
       <c r="J11" t="s">
         <v>2</v>
@@ -3503,7 +3504,7 @@
         <v>10</v>
       </c>
       <c r="L11">
-        <v>1961.51</v>
+        <v>1716.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>